<commit_message>
useful highlighting of forage_plant_location spreadsheet
</commit_message>
<xml_diff>
--- a/forage_plant_location.xlsx
+++ b/forage_plant_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0673F18-C311-EF49-9B4B-3C8BE5A98501}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA76F6D8-F761-E34C-9243-DB506339EEE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{B0640254-897E-44C3-B32E-9281997335F7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B0640254-897E-44C3-B32E-9281997335F7}"/>
   </bookViews>
   <sheets>
     <sheet name="forage_plant_location" sheetId="1" r:id="rId1"/>
@@ -686,8 +686,8 @@
   <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1297,7 +1297,7 @@
       <c r="G22" s="3">
         <v>0</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="13" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="14"/>
@@ -1540,7 +1540,7 @@
       <c r="G31" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="13" t="s">
         <v>15</v>
       </c>
       <c r="J31" s="14"/>
@@ -1729,7 +1729,7 @@
       <c r="G38" s="2">
         <v>1</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="13" t="s">
         <v>15</v>
       </c>
       <c r="J38" s="14"/>
@@ -1946,7 +1946,7 @@
       <c r="G46" s="2">
         <v>0</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="13" t="s">
         <v>15</v>
       </c>
       <c r="J46" s="15"/>
@@ -2027,7 +2027,7 @@
       <c r="G49" s="2">
         <v>0</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="13" t="s">
         <v>15</v>
       </c>
       <c r="J49" s="14"/>

</xml_diff>

<commit_message>
Finalise bee risk scores - 87/95 correct, but 8 incorrect appear to be due to Butler errors
</commit_message>
<xml_diff>
--- a/forage_plant_location.xlsx
+++ b/forage_plant_location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA76F6D8-F761-E34C-9243-DB506339EEE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24F8D02-EF47-6E41-A677-12278FD629FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B0640254-897E-44C3-B32E-9281997335F7}"/>
   </bookViews>
@@ -276,7 +276,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +301,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -314,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -361,6 +367,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,8 +695,8 @@
   <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -964,7 +973,7 @@
       <c r="D10" s="8">
         <v>1</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="18">
         <v>0</v>
       </c>
       <c r="F10" s="17">
@@ -1720,7 +1729,7 @@
       <c r="D38" s="2">
         <v>1</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="16">
         <v>0</v>
       </c>
       <c r="F38" s="2">

</xml_diff>